<commit_message>
Calendario de horas actualizado
Añadidas nuevas tareas, actualizadas las ya terminadas y reorganizado las horas y estimaciones. Añadida una leyenda de colores.
</commit_message>
<xml_diff>
--- a/CalendarioHorasTFG/TablaTFG.xlsx
+++ b/CalendarioHorasTFG/TablaTFG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\TFG\CalendarioHorasTFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F778AE2E-E3BD-4D07-9739-290AFCDF21E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3337125-9842-484F-9A69-D51EE67A2292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{844D4FD7-908D-4182-ACF1-14D636993B42}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>ID Tarea</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Implementación Hibernate</t>
-  </si>
-  <si>
     <t>Implementación API'S</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Estimación (aproximada)</t>
   </si>
   <si>
-    <t>Tiempo Empleado (Semanal)</t>
-  </si>
-  <si>
     <t>Lógica operaciones BBDD</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Lógica de el cálculo de estadísticas de juegos</t>
   </si>
   <si>
-    <t>Log in en la aplicación (Por decidir)</t>
-  </si>
-  <si>
     <t>Baja</t>
   </si>
   <si>
@@ -109,6 +100,27 @@
   </si>
   <si>
     <t>Pruebas</t>
+  </si>
+  <si>
+    <t>Tiempo Empleado (Diario)</t>
+  </si>
+  <si>
+    <t>Leyenda:</t>
+  </si>
+  <si>
+    <t>En curso</t>
+  </si>
+  <si>
+    <t>Pausada</t>
+  </si>
+  <si>
+    <t>Terminada</t>
+  </si>
+  <si>
+    <t>Implementación de log in (hash, cambiar pass…)</t>
+  </si>
+  <si>
+    <t>Exportación de biblioteca y wishlist</t>
   </si>
 </sst>
 </file>
@@ -133,7 +145,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +164,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,13 +189,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD959A5-F299-49B1-87BA-F7BCB5C02F52}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
@@ -510,10 +539,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -522,54 +551,54 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="10">
         <v>0.125</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E3" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="E4" s="10">
         <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -586,24 +615,24 @@
         <v>0.25</v>
       </c>
       <c r="E5" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="10">
         <v>0.10416666666666667</v>
       </c>
-      <c r="E6" s="4">
-        <v>2.0833333333333332E-2</v>
+      <c r="E6" s="10">
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -611,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -620,7 +649,7 @@
         <v>0.25</v>
       </c>
       <c r="E7" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -628,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -637,7 +666,7 @@
         <v>0.625</v>
       </c>
       <c r="E8" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -645,16 +674,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D9" s="4">
-        <v>0.625</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="E9" s="4">
-        <v>6.25E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -662,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -671,7 +700,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E10" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -679,16 +708,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E11" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -696,7 +725,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -705,7 +734,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E12" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -713,16 +742,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="E13" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -730,16 +759,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="4">
-        <v>0.625</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E14" s="4">
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -747,7 +776,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
@@ -756,7 +785,7 @@
         <v>0.625</v>
       </c>
       <c r="E15" s="4">
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -764,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
@@ -773,7 +802,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E16" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,7 +810,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
@@ -790,17 +819,31 @@
         <v>0.125</v>
       </c>
       <c r="E17" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" s="5">
-        <f>SUM(D2:D17)</f>
-        <v>5.3541666666666661</v>
+        <f>SUM(D5,D7:D17)</f>
+        <v>4.125</v>
       </c>
       <c r="E18" s="5">
-        <f>SUM(E2:E17)</f>
-        <v>0.57638888888888906</v>
+        <f>SUM(E5,E7:E17)</f>
+        <v>0.16666666666666669</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tablaTFG with the new estimated hours.
</commit_message>
<xml_diff>
--- a/CalendarioHorasTFG/TablaTFG.xlsx
+++ b/CalendarioHorasTFG/TablaTFG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\TFG\CalendarioHorasTFG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\app_tfg\CalendarioHorasTFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3337125-9842-484F-9A69-D51EE67A2292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009985A-1D3F-4835-99D4-1234D44B8429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{844D4FD7-908D-4182-ACF1-14D636993B42}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>ID Tarea</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Implementación API'S</t>
-  </si>
-  <si>
     <t>Implementación BBDD en código</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Lógica de el cálculo de estadísticas de juegos</t>
   </si>
   <si>
-    <t>Baja</t>
-  </si>
-  <si>
     <t>Docketización</t>
   </si>
   <si>
@@ -120,7 +114,10 @@
     <t>Implementación de log in (hash, cambiar pass…)</t>
   </si>
   <si>
-    <t>Exportación de biblioteca y wishlist</t>
+    <t>Exportación de biblioteca</t>
+  </si>
+  <si>
+    <t>Implementación API Videojuegos y Precios</t>
   </si>
 </sst>
 </file>
@@ -145,7 +142,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +173,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -189,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -201,6 +204,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +523,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,10 +544,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -602,20 +607,20 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="12">
         <v>0.25</v>
       </c>
-      <c r="E5" s="4">
-        <v>1.0416666666666666E-2</v>
+      <c r="E5" s="12">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -636,19 +641,19 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="10">
         <v>0.25</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="10">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
@@ -657,66 +662,66 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D8" s="4">
         <v>0.625</v>
       </c>
       <c r="E8" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="10">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="D11" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="10">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
@@ -725,7 +730,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -734,7 +739,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E12" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -742,16 +747,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D13" s="4">
         <v>0.375</v>
       </c>
       <c r="E13" s="4">
-        <v>1.0416666666666666E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -759,7 +764,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
@@ -768,7 +773,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E14" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -776,7 +781,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
@@ -793,7 +798,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
@@ -802,7 +807,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E16" s="4">
-        <v>6.9444444444444441E-3</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -810,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
@@ -824,26 +829,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" s="5">
-        <f>SUM(D5,D7:D17)</f>
-        <v>4.125</v>
+        <f>SUM(D5,D8,D12:D17)</f>
+        <v>3.041666666666667</v>
       </c>
       <c r="E18" s="5">
-        <f>SUM(E5,E7:E17)</f>
-        <v>0.16666666666666669</v>
+        <f>SUM(E5,E8,E12:E17)</f>
+        <v>0.27777777777777773</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed an error when a game doesn't have an image in the API, doesn't load the "ficha". Added the logic for stats (to be extended) and created the interface. Added a placeholder image when the api doesn't send an image for a videogame. Updated the "TablaTFG".
</commit_message>
<xml_diff>
--- a/CalendarioHorasTFG/TablaTFG.xlsx
+++ b/CalendarioHorasTFG/TablaTFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\app_tfg\CalendarioHorasTFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009985A-1D3F-4835-99D4-1234D44B8429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132E561-03EA-4927-A3B9-F569BB94E1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{844D4FD7-908D-4182-ACF1-14D636993B42}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>Docketización</t>
   </si>
   <si>
-    <t>Automatización para actualizar precios</t>
-  </si>
-  <si>
     <t>Documentación</t>
   </si>
   <si>
@@ -117,7 +114,10 @@
     <t>Exportación de biblioteca</t>
   </si>
   <si>
-    <t>Implementación API Videojuegos y Precios</t>
+    <t>Implementación API Videojuegos.</t>
+  </si>
+  <si>
+    <t>Refactorización de código, pequeños ajustes y quitar hardcode</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,12 +173,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -204,8 +198,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,12 +515,12 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.21875" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" customWidth="1"/>
     <col min="5" max="5" width="29.5546875" customWidth="1"/>
   </cols>
@@ -547,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -607,19 +599,19 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="12">
+      <c r="C5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10">
         <v>0.25</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -658,19 +650,19 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="10">
         <v>0.625</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -679,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>10</v>
@@ -726,19 +718,19 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -747,10 +739,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4">
         <v>0.375</v>
@@ -770,10 +762,10 @@
         <v>10</v>
       </c>
       <c r="D14" s="4">
-        <v>0.41666666666666669</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E14" s="4">
-        <v>6.25E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -781,13 +773,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D15" s="4">
-        <v>0.625</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="E15" s="4">
         <v>2.0833333333333332E-2</v>
@@ -798,13 +790,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4">
-        <v>0.20833333333333334</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E16" s="4">
         <v>2.0833333333333332E-2</v>
@@ -815,13 +807,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="4">
-        <v>0.125</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E17" s="4">
         <v>6.9444444444444441E-3</v>
@@ -829,26 +821,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" s="5">
-        <f>SUM(D5,D8,D12:D17)</f>
-        <v>3.041666666666667</v>
+        <f>SUM(D13:D17)</f>
+        <v>2.25</v>
       </c>
       <c r="E18" s="5">
-        <f>SUM(E5,E8,E12:E17)</f>
-        <v>0.27777777777777773</v>
+        <f>SUM(E13:E17)</f>
+        <v>0.17361111111111113</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created the method to export Biblbioteca to PDF. Added the dependency pdfbox, still refactoring the code.
</commit_message>
<xml_diff>
--- a/CalendarioHorasTFG/TablaTFG.xlsx
+++ b/CalendarioHorasTFG/TablaTFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\app_tfg\CalendarioHorasTFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132E561-03EA-4927-A3B9-F569BB94E1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC1D9EE-6340-4491-9E57-65D501D6ED98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{844D4FD7-908D-4182-ACF1-14D636993B42}"/>
   </bookViews>
@@ -515,7 +515,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="4">
-        <v>0.20833333333333334</v>
+        <v>0.625</v>
       </c>
       <c r="E15" s="4">
         <v>2.0833333333333332E-2</v>
@@ -822,7 +822,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" s="5">
         <f>SUM(D13:D17)</f>
-        <v>2.25</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="E18" s="5">
         <f>SUM(E13:E17)</f>

</xml_diff>